<commit_message>
I added a pie chart for practice
</commit_message>
<xml_diff>
--- a/data/Analysis.xlsx
+++ b/data/Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayemaq/Desktop/M0BusinessDataAnalysis_QureshiAyema/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F5576-4112-D143-B82C-48A11E468A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84347415-16ED-8E47-80D0-418849D2C756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A2CDBE70-898E-8C43-B2F1-42A296B50C1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A2CDBE70-898E-8C43-B2F1-42A296B50C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>Rate of Drop Off</t>
-  </si>
-  <si>
-    <t>Cart_Abandoned_Flag</t>
   </si>
 </sst>
 </file>
@@ -4431,6 +4428,37 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{297C97D2-BE57-7540-8C6B-07F2FC11ABE2}" name="Table1" displayName="Table1" ref="A1:P101" totalsRowShown="0">
+  <autoFilter ref="A1:P101" xr:uid="{297C97D2-BE57-7540-8C6B-07F2FC11ABE2}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{DE67F089-2F41-8A42-A2F8-DEE9F033221C}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{F06BBBFF-9A02-3344-8CD8-FB69AE66EBC7}" name="Is_Product_Details_viewed"/>
+    <tableColumn id="3" xr3:uid="{72DE0114-0DB5-6C49-A375-E299AF97902D}" name="Session_Activity_Count"/>
+    <tableColumn id="4" xr3:uid="{A4B3CBC8-51A6-284F-9673-1C7405E0E9F0}" name="No_Items_Added_InCart"/>
+    <tableColumn id="5" xr3:uid="{87905B28-4059-C34F-8D28-49EFE7ADEF4E}" name="No_Items_Removed_FromCart"/>
+    <tableColumn id="6" xr3:uid="{60AB05F0-7841-3749-BE42-63520ADA4FFA}" name="No_Cart_Viewed"/>
+    <tableColumn id="7" xr3:uid="{5D96DAA6-3597-B04F-A96A-1B18B272D418}" name="Purchase_Confirmed"/>
+    <tableColumn id="8" xr3:uid="{A4CCDF5F-896A-7B41-B61D-49D5B940C600}" name="Purchase_Initiated "/>
+    <tableColumn id="9" xr3:uid="{6A1BECFA-4DD3-4A44-B8FD-1CA77EFF4459}" name="No_Cart_Items_Viewed"/>
+    <tableColumn id="10" xr3:uid="{503B3E23-DA63-2941-BF7B-9143C1DC71C1}" name="No_Customer_Login"/>
+    <tableColumn id="11" xr3:uid="{4301838E-7F5D-8848-9692-8CB1D9C81E42}" name="No_Page_Viewed"/>
+    <tableColumn id="12" xr3:uid="{B9D998BB-DD10-CF49-8EC9-B6E5C8B58E7B}" name="Customer_Segment_Type"/>
+    <tableColumn id="13" xr3:uid="{1CEB61E4-AB80-6546-B01E-BF421FE8B2E3}" name="Cart_Abandoned"/>
+    <tableColumn id="14" xr3:uid="{384CF171-6672-0648-9D67-D7F8EDEF9BB9}" name="Added_items">
+      <calculatedColumnFormula>IF(ISNUMBER(D2), IF(D2 &gt; 0, "Yes", "No"), "No")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{C830B7F6-5533-E74E-8567-F104DBAA00BB}" name="Confirmed_Added_Items">
+      <calculatedColumnFormula>IF(N2 = "Yes", 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{2B63996A-8215-C147-83F4-8C8393249A1B}" name="Confirmed_iniated">
+      <calculatedColumnFormula>IF(H2 &gt;= 1, 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4750,33 +4778,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5ED015E-0EBC-0F42-AE6E-5A83AA63A374}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="106" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="106" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.5" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4825,11 +4854,8 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4882,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -4935,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4988,7 +5014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -5041,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -5094,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -5147,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -5200,7 +5226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -5253,7 +5279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5306,7 +5332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -5359,7 +5385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -5412,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -5465,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -5518,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5571,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -10131,6 +10157,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -10138,7 +10167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B202CC-2287-4B4F-A0DF-10B182779AF2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final updates: modified Analysis.xlsx and cleaned up files
</commit_message>
<xml_diff>
--- a/data/Analysis.xlsx
+++ b/data/Analysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayemaq/Desktop/M0BusinessDataAnalysis_QureshiAyema/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84347415-16ED-8E47-80D0-418849D2C756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9555A9F-6457-2345-A884-2E077F486EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A2CDBE70-898E-8C43-B2F1-42A296B50C1A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A2CDBE70-898E-8C43-B2F1-42A296B50C1A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -4780,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5ED015E-0EBC-0F42-AE6E-5A83AA63A374}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4949,11 +4949,11 @@
         <v>1</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N66" si="0">IF(ISNUMBER(D3), IF(D3 &gt; 0, "Yes", "No"), "No")</f>
+        <f>IF(ISNUMBER(D3), IF(D3 &gt; 0, "Yes", "No"), "No")</f>
         <v>No</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O66" si="1">IF(N3 = "Yes", 1, 0)</f>
+        <f t="shared" ref="O3:O66" si="0">IF(N3 = "Yes", 1, 0)</f>
         <v>0</v>
       </c>
       <c r="P3">
@@ -5002,11 +5002,11 @@
         <v>0</v>
       </c>
       <c r="N4" t="str">
+        <f t="shared" ref="N3:N66" si="1">IF(ISNUMBER(D4), IF(D4 &gt; 0, "Yes", "No"), "No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P4">
@@ -5055,11 +5055,11 @@
         <v>1</v>
       </c>
       <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5">
@@ -5108,11 +5108,11 @@
         <v>1</v>
       </c>
       <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P6">
@@ -5161,11 +5161,11 @@
         <v>1</v>
       </c>
       <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P7">
@@ -5214,11 +5214,11 @@
         <v>0</v>
       </c>
       <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P8">
@@ -5267,11 +5267,11 @@
         <v>1</v>
       </c>
       <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P9">
@@ -5320,11 +5320,11 @@
         <v>1</v>
       </c>
       <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P10">
@@ -5373,11 +5373,11 @@
         <v>0</v>
       </c>
       <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P11">
@@ -5430,7 +5430,7 @@
         <v>Yes</v>
       </c>
       <c r="O12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P12">
@@ -5479,11 +5479,11 @@
         <v>1</v>
       </c>
       <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P13">
@@ -5532,11 +5532,11 @@
         <v>1</v>
       </c>
       <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14">
@@ -5589,7 +5589,7 @@
         <v>No</v>
       </c>
       <c r="O15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P15">
@@ -5638,11 +5638,11 @@
         <v>1</v>
       </c>
       <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P16">
@@ -5691,11 +5691,11 @@
         <v>1</v>
       </c>
       <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O17">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P17">
@@ -5744,11 +5744,11 @@
         <v>1</v>
       </c>
       <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18">
@@ -5797,11 +5797,11 @@
         <v>1</v>
       </c>
       <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O19">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P19">
@@ -5850,11 +5850,11 @@
         <v>1</v>
       </c>
       <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O20">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P20">
@@ -5903,11 +5903,11 @@
         <v>1</v>
       </c>
       <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O21">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P21">
@@ -5956,11 +5956,11 @@
         <v>1</v>
       </c>
       <c r="N22" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O22">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P22">
@@ -6009,11 +6009,11 @@
         <v>1</v>
       </c>
       <c r="N23" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O23">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P23">
@@ -6062,11 +6062,11 @@
         <v>1</v>
       </c>
       <c r="N24" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O24">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P24">
@@ -6115,11 +6115,11 @@
         <v>1</v>
       </c>
       <c r="N25" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O25">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P25">
@@ -6168,11 +6168,11 @@
         <v>1</v>
       </c>
       <c r="N26" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O26">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P26">
@@ -6221,11 +6221,11 @@
         <v>1</v>
       </c>
       <c r="N27" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O27">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P27">
@@ -6274,11 +6274,11 @@
         <v>0</v>
       </c>
       <c r="N28" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O28">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P28">
@@ -6327,11 +6327,11 @@
         <v>0</v>
       </c>
       <c r="N29" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O29">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P29">
@@ -6380,11 +6380,11 @@
         <v>0</v>
       </c>
       <c r="N30" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O30">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P30">
@@ -6433,11 +6433,11 @@
         <v>1</v>
       </c>
       <c r="N31" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O31">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P31">
@@ -6486,11 +6486,11 @@
         <v>1</v>
       </c>
       <c r="N32" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O32">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P32">
@@ -6539,11 +6539,11 @@
         <v>1</v>
       </c>
       <c r="N33" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O33">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P33">
@@ -6592,11 +6592,11 @@
         <v>1</v>
       </c>
       <c r="N34" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O34">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P34">
@@ -6645,11 +6645,11 @@
         <v>1</v>
       </c>
       <c r="N35" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O35">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P35">
@@ -6698,11 +6698,11 @@
         <v>1</v>
       </c>
       <c r="N36" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O36">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O36">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P36">
@@ -6751,11 +6751,11 @@
         <v>1</v>
       </c>
       <c r="N37" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O37">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O37">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P37">
@@ -6804,11 +6804,11 @@
         <v>1</v>
       </c>
       <c r="N38" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O38">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O38">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P38">
@@ -6857,11 +6857,11 @@
         <v>1</v>
       </c>
       <c r="N39" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O39">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O39">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P39">
@@ -6910,11 +6910,11 @@
         <v>1</v>
       </c>
       <c r="N40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O40">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O40">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P40">
@@ -6963,11 +6963,11 @@
         <v>1</v>
       </c>
       <c r="N41" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O41">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O41">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P41">
@@ -7016,11 +7016,11 @@
         <v>1</v>
       </c>
       <c r="N42" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O42">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O42">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P42">
@@ -7069,11 +7069,11 @@
         <v>1</v>
       </c>
       <c r="N43" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O43">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O43">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P43">
@@ -7122,11 +7122,11 @@
         <v>1</v>
       </c>
       <c r="N44" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O44">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O44">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P44">
@@ -7175,11 +7175,11 @@
         <v>1</v>
       </c>
       <c r="N45" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O45">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O45">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P45">
@@ -7228,11 +7228,11 @@
         <v>0</v>
       </c>
       <c r="N46" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O46">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O46">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P46">
@@ -7281,11 +7281,11 @@
         <v>1</v>
       </c>
       <c r="N47" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O47">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O47">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P47">
@@ -7334,11 +7334,11 @@
         <v>0</v>
       </c>
       <c r="N48" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O48">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O48">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P48">
@@ -7387,11 +7387,11 @@
         <v>1</v>
       </c>
       <c r="N49" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O49">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O49">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P49">
@@ -7440,11 +7440,11 @@
         <v>1</v>
       </c>
       <c r="N50" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O50">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O50">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P50">
@@ -7493,11 +7493,11 @@
         <v>1</v>
       </c>
       <c r="N51" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O51">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O51">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P51">
@@ -7546,11 +7546,11 @@
         <v>1</v>
       </c>
       <c r="N52" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O52">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P52">
@@ -7599,11 +7599,11 @@
         <v>1</v>
       </c>
       <c r="N53" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O53">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O53">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P53">
@@ -7652,11 +7652,11 @@
         <v>1</v>
       </c>
       <c r="N54" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O54">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O54">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P54">
@@ -7705,11 +7705,11 @@
         <v>1</v>
       </c>
       <c r="N55" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="O55">
         <f t="shared" si="0"/>
-        <v>No</v>
-      </c>
-      <c r="O55">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P55">
@@ -7758,11 +7758,11 @@
         <v>1</v>
       </c>
       <c r="N56" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O56">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O56">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P56">
@@ -7811,11 +7811,11 @@
         <v>0</v>
       </c>
       <c r="N57" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O57">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O57">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P57">
@@ -7864,11 +7864,11 @@
         <v>1</v>
       </c>
       <c r="N58" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O58">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P58">
@@ -7917,11 +7917,11 @@
         <v>1</v>
       </c>
       <c r="N59" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O59">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O59">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P59">
@@ -7970,11 +7970,11 @@
         <v>1</v>
       </c>
       <c r="N60" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O60">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O60">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P60">
@@ -8023,11 +8023,11 @@
         <v>1</v>
       </c>
       <c r="N61" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O61">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O61">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P61">
@@ -8076,11 +8076,11 @@
         <v>1</v>
       </c>
       <c r="N62" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O62">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O62">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P62">
@@ -8129,11 +8129,11 @@
         <v>1</v>
       </c>
       <c r="N63" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O63">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O63">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P63">
@@ -8182,11 +8182,11 @@
         <v>1</v>
       </c>
       <c r="N64" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O64">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O64">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P64">
@@ -8235,11 +8235,11 @@
         <v>1</v>
       </c>
       <c r="N65" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O65">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O65">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P65">
@@ -8288,11 +8288,11 @@
         <v>1</v>
       </c>
       <c r="N66" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="O66">
         <f t="shared" si="0"/>
-        <v>Yes</v>
-      </c>
-      <c r="O66">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P66">
@@ -10167,8 +10167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B202CC-2287-4B4F-A0DF-10B182779AF2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>